<commit_message>
Menambah fitur CRUD PTK
</commit_message>
<xml_diff>
--- a/public/template/import_siswa.xlsx
+++ b/public/template/import_siswa.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\sidamas\public\template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\siak-foursma\public\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{257C2D24-0121-4800-B8E2-210DAC25B296}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01CABF28-5A9B-4F76-A2AF-1BA0EBE442C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B2D317BA-2D42-4279-940F-79954A4C82BF}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{B2D317BA-2D42-4279-940F-79954A4C82BF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>nisn</t>
   </si>
@@ -33,18 +33,55 @@
     <t>nama</t>
   </si>
   <si>
-    <t>siswa 1</t>
-  </si>
-  <si>
-    <t>0123456789</t>
+    <t>nis</t>
+  </si>
+  <si>
+    <t>nik</t>
+  </si>
+  <si>
+    <t>tempat lahir</t>
+  </si>
+  <si>
+    <t>tanggal lahir</t>
+  </si>
+  <si>
+    <t>jenis kelamin</t>
+  </si>
+  <si>
+    <t>agama</t>
+  </si>
+  <si>
+    <t>alamat</t>
+  </si>
+  <si>
+    <t>no hp</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>alamat orang tua</t>
+  </si>
+  <si>
+    <t>nama ayah</t>
+  </si>
+  <si>
+    <t>nama ibu</t>
+  </si>
+  <si>
+    <t>sekolah asal</t>
+  </si>
+  <si>
+    <t>tahun masuk</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="165" formatCode="mm/dd/yyyy"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -86,12 +123,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -407,7 +445,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F18DB8A8-C35B-48C1-BFBB-C96732606309}">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:P2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
@@ -416,32 +454,80 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12.44140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="43.6640625" customWidth="1"/>
-    <col min="3" max="3" width="9" style="1" customWidth="1"/>
-    <col min="4" max="4" width="9.88671875" customWidth="1"/>
-    <col min="5" max="5" width="9.6640625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="9.109375" customWidth="1"/>
-    <col min="7" max="7" width="9" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9" style="1" customWidth="1"/>
+    <col min="3" max="3" width="17.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22" style="2" customWidth="1"/>
+    <col min="5" max="5" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.109375" style="5" customWidth="1"/>
+    <col min="10" max="10" width="8.88671875" style="1"/>
+    <col min="16" max="16" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
         <v>1</v>
       </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>2</v>
-      </c>
-      <c r="J2" s="4"/>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A2" s="3"/>
+      <c r="D2"/>
+      <c r="I2" s="4"/>
     </row>
   </sheetData>
+  <dataValidations count="3">
+    <dataValidation showInputMessage="1" showErrorMessage="1" prompt="pastikan input tanggal dengan format dd/mm/yyy" sqref="F2:F1048576" xr:uid="{6725C3A8-B782-4840-A1F4-96F32940A9FF}"/>
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" prompt="Pilih jenis kelamin &quot;L&quot; untuk laki-laki atau &quot;P&quot; untuk perempuan" sqref="G2:G1048576" xr:uid="{5E4C6A35-AFC1-4278-AC38-35F765CAAB34}">
+      <formula1>"L,P"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Input tidak sesuai" prompt="Pilih agama : Hindu, Islam, Protestan, Katolik, Buddha, Konghubu" sqref="H2:H1048576" xr:uid="{2FC87F24-4929-44CA-B8EA-B644485AE257}">
+      <formula1>"Hindu,Islam,Protestan,KatoliklBuddha,Konghucu"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>